<commit_message>
added testdata into xl file, added enroll method with parametarization in helperclass
</commit_message>
<xml_diff>
--- a/Automation/src/test/java/Testdata/Testdata.xlsx
+++ b/Automation/src/test/java/Testdata/Testdata.xlsx
@@ -1,30 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/archana/Downloads/Automation-Framework/Automation/src/test/java/Testdata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView windowWidth="20490" windowHeight="7980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="addnetworkcenter" sheetId="1" r:id="rId1"/>
+    <sheet name="mychoosing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <oleSize ref="A1:F2"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>useremail</t>
   </si>
@@ -32,55 +24,443 @@
     <t>userpass</t>
   </si>
   <si>
+    <t>bussinessName</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>totaldailycost</t>
+  </si>
+  <si>
     <t>bhavya444@care.com</t>
   </si>
   <si>
     <t>letmein1</t>
   </si>
   <si>
-    <t>bussinessName</t>
-  </si>
-  <si>
-    <t>zipcode</t>
-  </si>
-  <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
-    <t>totaldailycost</t>
-  </si>
-  <si>
     <t>google</t>
   </si>
   <si>
+    <t>02451</t>
+  </si>
+  <si>
     <t>$2.20</t>
   </si>
   <si>
-    <t>02451</t>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>homeaddress</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Acm</t>
+  </si>
+  <si>
+    <t>04/22/1992</t>
+  </si>
+  <si>
+    <t>srinivas</t>
+  </si>
+  <si>
+    <t>Nelluri</t>
+  </si>
+  <si>
+    <t>P.O.Box 100</t>
+  </si>
+  <si>
+    <t>srinivas0244@care.com</t>
+  </si>
+  <si>
+    <t>Care</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -88,18 +468,308 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -152,7 +822,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -187,7 +857,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -361,32 +1031,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1666666666667" customWidth="1"/>
+    <col min="3" max="3" width="13.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="13.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,39 +1059,139 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E2">
         <v>9989089089</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="1"/>
+  <cols>
+    <col min="11" max="11" width="13.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>2541</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>8686101046</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="srinivas0244@care.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding hidekeyboard for typing
</commit_message>
<xml_diff>
--- a/Automation/src/test/java/Testdata/Testdata.xlsx
+++ b/Automation/src/test/java/Testdata/Testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="addnetworkcenter" sheetId="1" r:id="rId1"/>
@@ -1081,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,7 +1164,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>51</v>
+        <v>183</v>
       </c>
       <c r="I2" s="10">
         <v>2020</v>
@@ -1664,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:BG2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed the issues post updates in the testdata
</commit_message>
<xml_diff>
--- a/Automation/src/test/java/Testdata/Testdata.xlsx
+++ b/Automation/src/test/java/Testdata/Testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="addnetworkcenter" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="196">
   <si>
     <t>bhavya444@care.com</t>
   </si>
@@ -182,9 +182,6 @@
     <t>StarHealth</t>
   </si>
   <si>
-    <t>07</t>
-  </si>
-  <si>
     <t>from</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>P.O.Box 100</t>
   </si>
   <si>
-    <t>srinivas0244@care.com</t>
-  </si>
-  <si>
     <t>Care</t>
   </si>
   <si>
@@ -344,9 +338,6 @@
     <t>girl</t>
   </si>
   <si>
-    <t>2541</t>
-  </si>
-  <si>
     <t>enrollusername</t>
   </si>
   <si>
@@ -518,9 +509,6 @@
     <t>ycord</t>
   </si>
   <si>
-    <t>jags1@gmail.com</t>
-  </si>
-  <si>
     <t>123456789</t>
   </si>
   <si>
@@ -612,6 +600,21 @@
   </si>
   <si>
     <t>No allergies</t>
+  </si>
+  <si>
+    <t>03/21/2016</t>
+  </si>
+  <si>
+    <t>02541</t>
+  </si>
+  <si>
+    <t>srinivas012473@care.com</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>jags121456423@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -621,18 +624,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
     </font>
     <font>
       <u/>
@@ -770,15 +768,15 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -786,14 +784,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1081,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1095,23 +1092,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
@@ -1123,69 +1120,69 @@
         <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>9989089089</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="I2" s="10">
+      <c r="H2" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I2" s="9">
         <v>2020</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="J2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1195,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO10"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1218,11 +1215,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>9</v>
@@ -1234,10 +1231,10 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>12</v>
@@ -1315,54 +1312,54 @@
         <v>35</v>
       </c>
       <c r="AG1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="AI1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AJ1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AK1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AL1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AO1" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="AO1" s="12" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>51</v>
+        <v>194</v>
       </c>
       <c r="E2" s="4">
         <v>2020</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2" s="4">
         <v>9533679769</v>
@@ -1439,39 +1436,33 @@
       <c r="AF2" s="6">
         <v>87766554433</v>
       </c>
-      <c r="AG2" s="10" t="s">
+      <c r="AG2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI2" s="10" t="s">
+      <c r="AI2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AJ2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK2" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="AL2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AO2" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="D4" s="7"/>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="AI10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1481,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1495,72 +1486,74 @@
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" t="s">
-        <v>86</v>
-      </c>
       <c r="I1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K1" t="s">
         <v>11</v>
       </c>
       <c r="L1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" t="s">
         <v>96</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>97</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>98</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>99</v>
-      </c>
-      <c r="P1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>101</v>
       </c>
       <c r="R1" t="s">
         <v>2</v>
@@ -1574,40 +1567,46 @@
       <c r="U1" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W1" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="13" t="s">
-        <v>59</v>
+      <c r="X1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>88</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>90</v>
       </c>
-      <c r="E2" t="s">
-        <v>91</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>92</v>
+        <v>192</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>5</v>
+      <c r="I2" t="s">
+        <v>36</v>
       </c>
       <c r="J2">
         <v>15</v>
@@ -1615,26 +1614,26 @@
       <c r="K2">
         <v>2020</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>55</v>
+      <c r="L2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="N2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q2" t="s">
         <v>102</v>
       </c>
-      <c r="O2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" s="15">
-        <v>43221</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>104</v>
-      </c>
       <c r="R2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>8</v>
@@ -1645,11 +1644,17 @@
       <c r="U2" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="W2" s="9" t="s">
-        <v>61</v>
+      <c r="X2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1662,238 +1667,287 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG2"/>
+  <dimension ref="A1:BU2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>107</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>109</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>111</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>112</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>113</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>114</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>115</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>116</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>117</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>118</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>119</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>120</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>121</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>122</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>123</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>124</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>125</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>126</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>127</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>128</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>129</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>130</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>131</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>132</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>133</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>134</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>135</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>136</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>137</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>138</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>139</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>140</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>141</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP1" t="s">
         <v>142</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AQ1" t="s">
         <v>143</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AR1" t="s">
         <v>144</v>
       </c>
-      <c r="AN1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>145</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>146</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>147</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>148</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>149</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>150</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>151</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>152</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>153</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>154</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>155</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>156</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>157</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>158</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>159</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:73" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="C2" t="s">
         <v>161</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="D2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="E2" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J2" t="s">
         <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="L2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="N2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>8</v>
@@ -1902,19 +1956,19 @@
         <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="S2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="U2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>8</v>
@@ -1923,28 +1977,28 @@
         <v>37</v>
       </c>
       <c r="Y2" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC2" t="s">
         <v>176</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="AA2" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AF2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AG2">
         <v>87656787</v>
@@ -1953,7 +2007,7 @@
         <v>36</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="AJ2">
         <v>2020</v>
@@ -1961,47 +2015,47 @@
       <c r="AK2">
         <v>2</v>
       </c>
-      <c r="AL2" s="17" t="s">
+      <c r="AL2" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AP2" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AQ2" t="s">
         <v>185</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AR2" t="s">
         <v>186</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AS2" t="s">
         <v>187</v>
       </c>
-      <c r="AP2" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>189</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>190</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>191</v>
-      </c>
       <c r="AT2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AV2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="AZ2">
         <v>7</v>
@@ -2010,22 +2064,64 @@
         <v>0</v>
       </c>
       <c r="BB2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="BC2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="BD2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="BE2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="BH2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BI2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="BJ2" s="4">
+        <v>9533679769</v>
+      </c>
+      <c r="BK2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="BL2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="BQ2" s="4">
+        <v>9533679769</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="BT2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the reportportal integration code
</commit_message>
<xml_diff>
--- a/Automation/src/test/java/Testdata/Testdata.xlsx
+++ b/Automation/src/test/java/Testdata/Testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="addnetworkcenter" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="196">
   <si>
     <t>bhavya444@care.com</t>
   </si>
@@ -137,9 +137,6 @@
     <t>policyNumber</t>
   </si>
   <si>
-    <t>May</t>
-  </si>
-  <si>
     <t>Mother</t>
   </si>
   <si>
@@ -566,12 +563,6 @@
     <t>stateinsurance</t>
   </si>
   <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09:00 AM</t>
-  </si>
-  <si>
     <t>05:00 PM</t>
   </si>
   <si>
@@ -608,13 +599,22 @@
     <t>02541</t>
   </si>
   <si>
-    <t>srinivas012473@care.com</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>jags121456423@gmail.com</t>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>srinivas0124768532@care.com</t>
+  </si>
+  <si>
+    <t>jags125678435@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,22 +1093,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
@@ -1120,22 +1120,22 @@
         <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="N1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1158,31 +1158,31 @@
         <v>7</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="I2" s="9">
         <v>2020</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="N2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:W2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,10 +1216,10 @@
   <sheetData>
     <row r="1" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>9</v>
@@ -1231,10 +1231,10 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>12</v>
@@ -1312,31 +1312,31 @@
         <v>35</v>
       </c>
       <c r="AG1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AH1" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="AI1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AK1" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="AL1" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AM1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="AO1" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1347,121 +1347,121 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E2" s="4">
         <v>2020</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="4">
         <v>9533679769</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="L2" s="4">
         <v>9533679769</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="S2" s="4">
         <v>9533679769</v>
       </c>
       <c r="T2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y2" s="4">
         <v>9533679769</v>
       </c>
       <c r="Z2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="AD2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AF2" s="6">
         <v>87766554433</v>
       </c>
       <c r="AG2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AH2" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="AI2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AJ2" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK2" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="AL2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1475,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1485,8 +1485,8 @@
     <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
@@ -1505,55 +1505,55 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>84</v>
       </c>
-      <c r="H1" t="s">
-        <v>85</v>
-      </c>
       <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
         <v>92</v>
-      </c>
-      <c r="J1" t="s">
-        <v>93</v>
       </c>
       <c r="K1" t="s">
         <v>11</v>
       </c>
       <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>95</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>97</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>98</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>99</v>
       </c>
       <c r="R1" t="s">
         <v>2</v>
@@ -1568,72 +1568,72 @@
         <v>5</v>
       </c>
       <c r="V1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" t="s">
         <v>57</v>
       </c>
-      <c r="W1" t="s">
-        <v>58</v>
-      </c>
       <c r="X1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2">
-        <v>15</v>
-      </c>
-      <c r="K2">
-        <v>2020</v>
+        <v>191</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" t="s">
         <v>100</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q2" t="s">
         <v>101</v>
       </c>
-      <c r="P2" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>102</v>
-      </c>
       <c r="R2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>8</v>
@@ -1645,16 +1645,16 @@
         <v>7</v>
       </c>
       <c r="V2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="X2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1669,13 +1669,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="9.83203125" bestFit="1" customWidth="1"/>
@@ -1684,181 +1704,181 @@
   <sheetData>
     <row r="1" spans="1:73" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>105</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>111</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>112</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>113</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>114</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>115</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>116</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>117</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>119</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>120</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>121</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>122</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>123</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>124</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>125</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>126</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>127</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>128</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>129</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>130</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>131</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>132</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>133</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>134</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>135</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>136</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>137</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>138</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>139</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>140</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP1" t="s">
         <v>141</v>
       </c>
-      <c r="AN1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>142</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>143</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>144</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>145</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>146</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>147</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>148</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>149</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>150</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>151</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>152</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>153</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>154</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>155</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>156</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>157</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>158</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>159</v>
       </c>
       <c r="BH1" s="2" t="s">
         <v>14</v>
@@ -1908,106 +1928,106 @@
         <v>195</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
         <v>160</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>161</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" t="s">
         <v>165</v>
       </c>
-      <c r="J2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>166</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O2" t="s">
         <v>168</v>
-      </c>
-      <c r="N2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O2" t="s">
-        <v>169</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R2" t="s">
+        <v>169</v>
+      </c>
+      <c r="S2" t="s">
+        <v>165</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="S2" t="s">
-        <v>166</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="U2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="X2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y2" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AB2" t="s">
         <v>174</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>175</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AF2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG2">
         <v>87656787</v>
       </c>
-      <c r="AH2" t="s">
-        <v>36</v>
+      <c r="AH2" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="AJ2">
         <v>2020</v>
@@ -2016,46 +2036,46 @@
         <v>2</v>
       </c>
       <c r="AL2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AO2" t="s">
         <v>180</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AP2" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AQ2" t="s">
         <v>182</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AR2" t="s">
         <v>183</v>
       </c>
-      <c r="AP2" s="15" t="s">
+      <c r="AS2" t="s">
         <v>184</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>185</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>186</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>187</v>
-      </c>
       <c r="AT2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AV2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AZ2">
         <v>7</v>
@@ -2064,64 +2084,64 @@
         <v>0</v>
       </c>
       <c r="BB2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="BC2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BE2" t="s">
         <v>150</v>
       </c>
-      <c r="BD2" t="s">
-        <v>150</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>151</v>
-      </c>
       <c r="BF2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BH2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="BI2" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="BI2" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="BJ2" s="4">
         <v>9533679769</v>
       </c>
       <c r="BK2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="BL2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="BL2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="BM2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="BN2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="BO2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BO2" s="4" t="s">
+      <c r="BP2" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="BP2" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="BQ2" s="4">
         <v>9533679769</v>
       </c>
       <c r="BR2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="BS2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="BS2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="BT2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="BU2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>